<commit_message>
Bug Fix - "Torp to Energy" and "Energy to Torp" add Shift key to get CAP "U" and "I"
</commit_message>
<xml_diff>
--- a/KeyMappings.xlsx
+++ b/KeyMappings.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adamsb\Google Drive\LMN-Brian\Artemis\New Firmware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MFlaga\Google Drive\Arduino\Artemis23consoleMultiJoyStick\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="10650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="210">
   <si>
     <t>Console</t>
   </si>
@@ -648,6 +648,12 @@
   </si>
   <si>
     <t>0x23</t>
+  </si>
+  <si>
+    <t>Shift+U</t>
+  </si>
+  <si>
+    <t>Shift+I</t>
   </si>
 </sst>
 </file>
@@ -967,18 +973,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.54296875" customWidth="1"/>
-    <col min="2" max="2" width="15.81640625" customWidth="1"/>
-    <col min="5" max="5" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1001,7 +1007,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1021,7 +1027,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1041,7 +1047,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1061,7 +1067,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1081,7 +1087,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1101,7 +1107,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1121,7 +1127,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1141,7 +1147,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1161,7 +1167,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1181,7 +1187,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1201,7 +1207,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1221,7 +1227,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -1241,7 +1247,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1261,7 +1267,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -1281,7 +1287,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -1301,7 +1307,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1321,7 +1327,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -1341,7 +1347,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -1361,7 +1367,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1381,7 +1387,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1401,7 +1407,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -1421,7 +1427,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -1441,7 +1447,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -1461,7 +1467,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -1481,7 +1487,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -1501,7 +1507,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -1521,7 +1527,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -1541,7 +1547,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -1561,7 +1567,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>55</v>
       </c>
@@ -1581,7 +1587,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>55</v>
       </c>
@@ -1601,7 +1607,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>55</v>
       </c>
@@ -1618,7 +1624,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>55</v>
       </c>
@@ -1635,7 +1641,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>55</v>
       </c>
@@ -1652,7 +1658,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>55</v>
       </c>
@@ -1672,7 +1678,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>55</v>
       </c>
@@ -1692,7 +1698,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>55</v>
       </c>
@@ -1712,7 +1718,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>55</v>
       </c>
@@ -1726,13 +1732,13 @@
         <v>8</v>
       </c>
       <c r="E38" t="s">
-        <v>92</v>
+        <v>208</v>
       </c>
       <c r="F38" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>55</v>
       </c>
@@ -1746,13 +1752,13 @@
         <v>9</v>
       </c>
       <c r="E39" t="s">
-        <v>93</v>
+        <v>209</v>
       </c>
       <c r="F39" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>55</v>
       </c>
@@ -1775,7 +1781,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>55</v>
       </c>
@@ -1798,7 +1804,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>55</v>
       </c>
@@ -1821,7 +1827,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>55</v>
       </c>
@@ -1844,7 +1850,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>55</v>
       </c>
@@ -1867,7 +1873,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>55</v>
       </c>
@@ -1890,7 +1896,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>55</v>
       </c>
@@ -1913,7 +1919,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>55</v>
       </c>
@@ -1936,7 +1942,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>55</v>
       </c>
@@ -1956,7 +1962,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>55</v>
       </c>
@@ -1976,7 +1982,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>55</v>
       </c>
@@ -1996,7 +2002,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>55</v>
       </c>
@@ -2016,7 +2022,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>55</v>
       </c>
@@ -2036,7 +2042,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>55</v>
       </c>
@@ -2056,7 +2062,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>55</v>
       </c>
@@ -2076,7 +2082,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -2096,7 +2102,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -2116,7 +2122,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -2136,7 +2142,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>55</v>
       </c>
@@ -2156,7 +2162,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>55</v>
       </c>
@@ -2176,7 +2182,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>55</v>
       </c>
@@ -2196,7 +2202,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>55</v>
       </c>
@@ -2216,7 +2222,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>108</v>
       </c>
@@ -2236,7 +2242,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>108</v>
       </c>
@@ -2256,7 +2262,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>108</v>
       </c>
@@ -2276,7 +2282,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>108</v>
       </c>
@@ -2296,7 +2302,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>108</v>
       </c>
@@ -2313,7 +2319,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>108</v>
       </c>
@@ -2330,7 +2336,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>150</v>
       </c>
@@ -2350,7 +2356,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>150</v>
       </c>
@@ -2370,7 +2376,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>150</v>
       </c>
@@ -2390,7 +2396,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>150</v>
       </c>
@@ -2410,7 +2416,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>150</v>
       </c>
@@ -2430,7 +2436,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>150</v>
       </c>
@@ -2450,7 +2456,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>150</v>
       </c>
@@ -2470,7 +2476,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>150</v>
       </c>
@@ -2490,7 +2496,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>150</v>
       </c>
@@ -2510,7 +2516,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>150</v>
       </c>
@@ -2530,7 +2536,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>150</v>
       </c>
@@ -2550,7 +2556,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>150</v>
       </c>
@@ -2570,7 +2576,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>173</v>
       </c>
@@ -2590,7 +2596,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>173</v>
       </c>
@@ -2610,7 +2616,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>173</v>
       </c>
@@ -2630,7 +2636,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>173</v>
       </c>
@@ -2650,7 +2656,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>173</v>
       </c>
@@ -2670,7 +2676,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>173</v>
       </c>
@@ -2690,7 +2696,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>173</v>
       </c>
@@ -2710,7 +2716,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>173</v>
       </c>
@@ -2730,7 +2736,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>173</v>
       </c>
@@ -2750,7 +2756,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>173</v>
       </c>
@@ -2770,7 +2776,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>173</v>
       </c>
@@ -2790,7 +2796,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>6</v>
       </c>
@@ -2810,7 +2816,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>6</v>
       </c>
@@ -2830,7 +2836,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>6</v>
       </c>
@@ -2850,7 +2856,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>6</v>
       </c>
@@ -2870,7 +2876,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>6</v>
       </c>
@@ -2890,7 +2896,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>6</v>
       </c>
@@ -2910,7 +2916,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>6</v>
       </c>
@@ -2930,7 +2936,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>6</v>
       </c>
@@ -2950,7 +2956,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>6</v>
       </c>
@@ -2970,7 +2976,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>6</v>
       </c>
@@ -2984,7 +2990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>6</v>
       </c>
@@ -2998,7 +3004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>6</v>
       </c>
@@ -3012,7 +3018,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>6</v>
       </c>
@@ -3032,7 +3038,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>6</v>
       </c>
@@ -3052,7 +3058,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>6</v>
       </c>
@@ -3072,7 +3078,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>6</v>
       </c>
@@ -3092,7 +3098,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>6</v>
       </c>
@@ -3112,7 +3118,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>6</v>
       </c>
@@ -3132,7 +3138,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>6</v>
       </c>
@@ -3152,7 +3158,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>6</v>
       </c>
@@ -3172,7 +3178,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>6</v>
       </c>
@@ -3180,7 +3186,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>6</v>
       </c>
@@ -3188,7 +3194,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>6</v>
       </c>
@@ -3196,7 +3202,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>6</v>
       </c>
@@ -3216,7 +3222,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>6</v>
       </c>
@@ -3236,7 +3242,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Bug Fix - corrected Zoom In/Out buttons for Science
</commit_message>
<xml_diff>
--- a/KeyMappings.xlsx
+++ b/KeyMappings.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="214">
   <si>
     <t>Console</t>
   </si>
@@ -654,6 +654,18 @@
   </si>
   <si>
     <t>Shift+I</t>
+  </si>
+  <si>
+    <t>Arrow Up</t>
+  </si>
+  <si>
+    <t>Arro Down</t>
+  </si>
+  <si>
+    <t>0xDA</t>
+  </si>
+  <si>
+    <t>0xD9</t>
   </si>
 </sst>
 </file>
@@ -973,8 +985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2315,8 +2327,11 @@
       <c r="D66">
         <v>6</v>
       </c>
+      <c r="E66" t="s">
+        <v>210</v>
+      </c>
       <c r="F66" t="s">
-        <v>172</v>
+        <v>212</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -2332,8 +2347,11 @@
       <c r="D67">
         <v>5</v>
       </c>
+      <c r="E67" t="s">
+        <v>211</v>
+      </c>
       <c r="F67" t="s">
-        <v>172</v>
+        <v>213</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>